<commit_message>
Task graph metrics presentation
</commit_message>
<xml_diff>
--- a/Notes/TaskGraphMetrics-EdgeDetect.xlsx
+++ b/Notes/TaskGraphMetrics-EdgeDetect.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Dev\Experiments\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74A3FF3-0F7E-41EB-8E27-F40898CB9B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFBB18E-BAF7-49DD-BD3F-35F2AC1D4294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>